<commit_message>
Completed the version submitted to Canvas.
</commit_message>
<xml_diff>
--- a/Report/methods.xlsx
+++ b/Report/methods.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clayton\Documents\University\Fifta_Gear\Forma_Siexmonaþ\ELEC4840A\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F970B08C-8078-46D2-9F81-733B413E2B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1338406-AE19-4273-955C-7910951EDDEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{07585544-E12D-4E46-AE8C-97FC665E4C93}"/>
   </bookViews>
@@ -826,8 +826,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EEC962C-60BA-403A-8713-E755FAE596A7}">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -838,12 +838,11 @@
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.08203125" customWidth="1"/>
-    <col min="7" max="7" width="9.4140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.4140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.4140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.4140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.4140625" customWidth="1"/>
+    <col min="7" max="7" width="9.4140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="7.4140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="7.4140625" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="11.4140625" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.25" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="48.58203125" bestFit="1" customWidth="1"/>

</xml_diff>